<commit_message>
Add xlsm file to support macro
</commit_message>
<xml_diff>
--- a/ChartAPITest.xlsx
+++ b/ChartAPITest.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" activeTab="1" xr2:uid="{48C69550-37B8-49E9-864A-547F883FAADA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{48C69550-37B8-49E9-864A-547F883FAADA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bubble" sheetId="1" r:id="rId1"/>
     <sheet name="Line" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -124,15 +124,18 @@
       <c:bubbleChart>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Product B</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
+              <a:schemeClr val="accent2">
                 <a:alpha val="75000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
@@ -140,28 +143,49 @@
           <c:invertIfNegative val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Bubble!$F$3:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Bubble!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>Bubble!$H$3:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -172,31 +196,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:bubbleSize>
-            <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -204,7 +207,7 @@
           <c:bubble3D val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D1B6-441F-B542-C520085368BD}"/>
+              <c16:uniqueId val="{00000001-9441-4A09-9F33-2123266AF748}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -218,11 +221,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="926488208"/>
-        <c:axId val="923190848"/>
+        <c:axId val="1403303584"/>
+        <c:axId val="1368434720"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="926488208"/>
+        <c:axId val="1403303584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,12 +282,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="923190848"/>
+        <c:crossAx val="1368434720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="923190848"/>
+        <c:axId val="1368434720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="926488208"/>
+        <c:crossAx val="1403303584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1888,23 +1891,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B34BB2AB-185A-40B4-88A5-49859697E3F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8AE27EA-49CB-4203-8396-4B434A54B167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2263,7 +2266,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="616" row="4">
+  <wetp:taskpane dockstate="right" visibility="0" width="758" row="4">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2283,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B488C89-B7DD-4D99-BBE4-34F2365D6D63}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B649B0F-696D-47C7-AFF4-249D2478C984}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>

</xml_diff>